<commit_message>
Primeira parte da freight table proveniente de pdf
Com ajuda do pacote tabulizer, tive de delimitar a área desejada e selecionar a página do documento, pdf o que poderá comprometer o algoritmo em produção.
</commit_message>
<xml_diff>
--- a/duf_freight_table.xlsx
+++ b/duf_freight_table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C4D581-AC2C-4BDB-A28E-9DD87CBE8C9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{DCD60E1A-F264-43E3-A08B-21F8235C49CF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12800" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="9600" windowWidth="12800" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -107,17 +107,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="3">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -415,80 +416,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>destination_geographic_identifier</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>range_end</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>minimum_freight</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>invoice_factor</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>weight_factor</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>base_freight_cost</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>percentage_invoice</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>exceeding_weight_cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ES-Capital</t>
+        </is>
       </c>
       <c r="C2" s="1">
-        <v>46.012999999999998</v>
+        <v>46.013</v>
       </c>
       <c r="D2" s="1">
         <v>1.49</v>
       </c>
       <c r="E2" s="1">
-        <v>0.39600000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
+        <v>0.396</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ES-Interior 1</t>
+        </is>
       </c>
       <c r="C3" s="1">
-        <v>59.026000000000003</v>
+        <v>59.026</v>
       </c>
       <c r="D3" s="1">
         <v>1.73</v>
       </c>
       <c r="E3" s="1">
-        <v>0.51700000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>10</v>
+        <v>0.517</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>RJ-Capital 1</t>
+        </is>
       </c>
       <c r="C4" s="1">
         <v>48.73</v>
@@ -497,12 +508,14 @@
         <v>1.49</v>
       </c>
       <c r="E4" s="1">
-        <v>0.39600000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>11</v>
+        <v>0.396</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>RJ-Interior 1</t>
+        </is>
       </c>
       <c r="C5" s="1">
         <v>60.5</v>
@@ -511,12 +524,14 @@
         <v>1.73</v>
       </c>
       <c r="E5" s="1">
-        <v>0.60499999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
+        <v>0.605</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SP-Capital</t>
+        </is>
       </c>
       <c r="C6" s="1">
         <v>48.24</v>
@@ -528,9 +543,11 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>13</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SP-Interior 1</t>
+        </is>
       </c>
       <c r="C7" s="1">
         <v>77</v>
@@ -542,23 +559,27 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ES-Interior 2</t>
+        </is>
       </c>
       <c r="C8" s="1">
-        <v>59.026000000000003</v>
+        <v>59.026</v>
       </c>
       <c r="D8" s="1">
         <v>1.73</v>
       </c>
       <c r="E8" s="1">
-        <v>0.51700000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>15</v>
+        <v>0.517</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RJ-Capital 2</t>
+        </is>
       </c>
       <c r="C9" s="1">
         <v>48.73</v>
@@ -567,12 +588,14 @@
         <v>1.49</v>
       </c>
       <c r="E9" s="1">
-        <v>0.39600000000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>16</v>
+        <v>0.396</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>RJ-Interior 2</t>
+        </is>
       </c>
       <c r="C10" s="1">
         <v>60.5</v>
@@ -581,12 +604,14 @@
         <v>1.73</v>
       </c>
       <c r="E10" s="1">
-        <v>0.60499999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>17</v>
+        <v>0.605</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SP-Interior 2</t>
+        </is>
       </c>
       <c r="C11" s="1">
         <v>77</v>
@@ -599,6 +624,5 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>